<commit_message>
Update visibility criteria to use data element IDs instead of component codes
</commit_message>
<xml_diff>
--- a/packages/lan/data/demo_survey.xlsx
+++ b/packages/lan/data/demo_survey.xlsx
@@ -252,7 +252,7 @@
     <t xml:space="preserve">Ongoing Condition, Drug Therapy</t>
   </si>
   <si>
-    <t xml:space="preserve">TamanuProgramsTest14: Yes</t>
+    <t xml:space="preserve">TamanuProgramsTest16: Yes</t>
   </si>
   <si>
     <t xml:space="preserve">TamanuProgramsTest18</t>
@@ -374,8 +374,8 @@
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,7 +384,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="86.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>